<commit_message>
Carrera para listado de ETS
</commit_message>
<xml_diff>
--- a/src/main/java/com/example/PruebaCRUD/grupos_ESCOM.xlsx
+++ b/src/main/java/com/example/PruebaCRUD/grupos_ESCOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alfre\OneDrive\Documentos\Semestres ESCOM\Semestre 7 - ESCOM\Control-Acceso\Programas\SpringBoot-Java\src\main\java\com\example\PruebaCRUD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0893A8C5-1660-4F81-958B-BB390AB1430E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B577F5-BCE3-42E1-82EC-3E7D9A8A1544}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" activeTab="1" xr2:uid="{C2E9D6F7-9EB6-5048-BE23-0181DDD0E157}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" activeTab="3" xr2:uid="{C2E9D6F7-9EB6-5048-BE23-0181DDD0E157}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1132,10 +1132,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{229E4F30-96FB-2146-BEE0-A03B8B16FF49}">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
@@ -1850,6 +1850,16 @@
         <v>125</v>
       </c>
     </row>
+    <row r="38" spans="3:3">
+      <c r="C38">
+        <v>2022630147</v>
+      </c>
+    </row>
+    <row r="39" spans="3:3">
+      <c r="C39">
+        <v>2024630445</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1860,7 +1870,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98534562-AC4B-244A-A57F-3BC18AA9C42E}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -2377,8 +2387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65FB40E8-2696-B44B-9363-8A04EE70803A}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10:F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
@@ -3071,12 +3081,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="dcba946b-1e56-43c3-ba83-7d0b5c0830eb">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7dc027c4-69c3-486d-8dac-5c643ba62fa0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3275,20 +3287,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="dcba946b-1e56-43c3-ba83-7d0b5c0830eb">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7dc027c4-69c3-486d-8dac-5c643ba62fa0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D592D51E-05C2-446D-A236-0D92EE0ED833}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D288AF6C-10A4-4C12-B6A3-B6A78DD62184}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="dcba946b-1e56-43c3-ba83-7d0b5c0830eb"/>
+    <ds:schemaRef ds:uri="7dc027c4-69c3-486d-8dac-5c643ba62fa0"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3313,12 +3326,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D288AF6C-10A4-4C12-B6A3-B6A78DD62184}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D592D51E-05C2-446D-A236-0D92EE0ED833}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="dcba946b-1e56-43c3-ba83-7d0b5c0830eb"/>
-    <ds:schemaRef ds:uri="7dc027c4-69c3-486d-8dac-5c643ba62fa0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>